<commit_message>
fixes to AllocatedIntake class and to remove double-counting of shared infrastructure capacity coming online, plus fixes to variable allocation change deltas and tweak of unit cost objective
</commit_message>
<xml_diff>
--- a/DV_Objective_Documentation.xlsx
+++ b/DV_Objective_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dgorelic_ad_unc_edu/Documents/UNC/Research/WSC/Coding/WP/WaterPaths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="249" documentId="8_{C446E435-FD69-48B3-871F-E429E1FF7D24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BDBD410F-FF78-461C-971C-F32CF511BE2A}"/>
+  <xr:revisionPtr revIDLastSave="267" documentId="8_{C446E435-FD69-48B3-871F-E429E1FF7D24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BF9B272A-7216-456C-B395-D3F18F1F50C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F54973CA-8AA1-40B0-98EE-38B94B0F6783}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F54973CA-8AA1-40B0-98EE-38B94B0F6783}"/>
   </bookViews>
   <sheets>
     <sheet name="DVs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
   <si>
     <t>Unit</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Average across realizations of present-valued debt service costs between 2015-2060 divided by total water demand over same period</t>
   </si>
   <si>
-    <t>$MM/MG</t>
-  </si>
-  <si>
     <t>fraction of AVR</t>
   </si>
   <si>
@@ -291,6 +288,24 @@
   </si>
   <si>
     <t>fixed by project</t>
+  </si>
+  <si>
+    <t>$/kgal</t>
+  </si>
+  <si>
+    <t>Suggested BORG Spacing</t>
+  </si>
+  <si>
+    <t>precise to 500-step space, given 1,000 realizations</t>
+  </si>
+  <si>
+    <t>equates to $1 million increments</t>
+  </si>
+  <si>
+    <t>equates to increments of 1% of annual revenue</t>
+  </si>
+  <si>
+    <t>equates to $0.01 (one cent) increments</t>
   </si>
 </sst>
 </file>
@@ -347,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -366,6 +381,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E8025B-B80B-4FCF-84DB-917353BEAF4C}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -904,13 +920,13 @@
         <v>35</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -998,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74835E3A-F5AB-4290-9E88-38EA5BFCB9C6}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,9 +1025,10 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1024,8 +1041,13 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -1038,8 +1060,14 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>2E-3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1052,8 +1080,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
@@ -1066,8 +1097,14 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
@@ -1075,13 +1112,19 @@
         <v>70</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
@@ -1089,13 +1132,16 @@
         <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
@@ -1103,10 +1149,16 @@
         <v>73</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="E7">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1118,7 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E77D40-9854-4509-89AE-89F935EB7189}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1145,7 +1197,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
@@ -1156,7 +1208,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>0.05</v>
@@ -1164,32 +1216,32 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
         <v>83</v>
-      </c>
-      <c r="D6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1415,18 +1467,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1449,26 +1501,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{727DE186-B72B-4CD9-90D9-A8454155DDF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8692fb02-64ee-477a-8829-0b8419474116"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e525f45e-12aa-43f1-99a0-18fd9df9a174"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B90AB10-682F-4A2A-B62D-D34EDE2A9D91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{727DE186-B72B-4CD9-90D9-A8454155DDF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8692fb02-64ee-477a-8829-0b8419474116"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e525f45e-12aa-43f1-99a0-18fd9df9a174"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>